<commit_message>
Added stature data to data list
</commit_message>
<xml_diff>
--- a/docs/data/stature.xlsx
+++ b/docs/data/stature.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\docs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200440AC-43F2-4779-8B45-0F4BE853E032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49F56757-3482-47E0-88AE-508EBDC5E43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{B2857A61-B0A5-4841-A0B4-1BE680B214C2}"/>
   </bookViews>

</xml_diff>